<commit_message>
Ultimos cambios para presentacion
</commit_message>
<xml_diff>
--- a/Agronomunnity/static/temp/bitacora.xlsx
+++ b/Agronomunnity/static/temp/bitacora.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Bitacora de reportes del 26 de mayo de 2023 al 29 de mayo de 2023</t>
+          <t>Bitacora de reportes del 26 de mayo de 2023 al 01 de junio de 2023</t>
         </is>
       </c>
     </row>
@@ -680,16 +680,16 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="n">
-        <v>45075</v>
+        <v>45078</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Huertas del mirador</t>
+          <t>Huerta Sierra Madre</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Rodrigo Sebastian Villaseñor Cornejo</t>
+          <t>Pedro Mendoza Cobarrubias</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -699,34 +699,34 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Gasolinera Ejido Opopeo</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mercedes Benz / Freightliner Cascadia Clásica</t>
+          <t>H-2345</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Alan Garcia Diaz</t>
+          <t>Ruben Juarez Hernandez</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Cuadrilla del sur</t>
+          <t>Cuadrilla Michoacanos</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>F2DS32</t>
+          <t>HINO12321</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>6800</v>
+        <v>10000</v>
       </c>
       <c r="K9" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -735,157 +735,94 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>San Diego, Californi</t>
+          <t>Phoenix, Arizona</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Cliente de mostrador</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr"/>
+          <t>Kevin Morales  Tellez</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>El pedido debe enviar un regalo</t>
+        </is>
+      </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="n">
-        <v>45075</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Huertas del mirador</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Rodrigo Sebastian Villaseñor Cornejo</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Aventajado</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Mercedes Benz / Freightliner Cascadia Clásica</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Alan Garcia Diaz</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Cuadrilla los potrillos</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>F2DS32</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>2500</v>
-      </c>
-      <c r="K10" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Tepic, Nayarit</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Cliente de mostrador</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
+    <row r="12">
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>PRECIOS AUTORIZADOS</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>FRUTA DE HUERTAS</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>PRECIOS AUTORIZADOS</t>
-        </is>
-      </c>
-      <c r="I13" s="5" t="inlineStr">
-        <is>
-          <t>FRUTA DE HUERTAS</t>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>ESTADO</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>DESCRIPCION</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>PRECIO</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>VIGENCIA</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>HUERTA</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>FRUTA</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>PRECIO</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>ESTADO</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>DESCRIPCION</t>
-        </is>
-      </c>
-      <c r="E14" s="3" t="inlineStr">
-        <is>
-          <t>PRECIO</t>
-        </is>
-      </c>
-      <c r="F14" s="3" t="inlineStr">
-        <is>
-          <t>VIGENCIA</t>
-        </is>
-      </c>
-      <c r="I14" s="3" t="inlineStr">
-        <is>
-          <t>HUERTA</t>
-        </is>
-      </c>
-      <c r="J14" s="3" t="inlineStr">
-        <is>
-          <t>FRUTA</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>PRECIO</t>
-        </is>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Oaxaca</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Precio de aguacate Hass</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>25.124</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>45577</v>
       </c>
     </row>
-    <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Oaxaca</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Precio de aguacate Hass</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>25.124</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <v>45577</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="6" t="inlineStr">
+    <row r="17">
+      <c r="C17" s="6" t="inlineStr">
         <is>
           <t>Precios Autorizados por Gustavo Garcia Rodriguez.</t>
         </is>
       </c>
-      <c r="H18" s="6" t="inlineStr">
+      <c r="H17" s="6" t="inlineStr">
         <is>
           <t>Bitacora generada por Jonathan Juarez Hernandez.</t>
         </is>
@@ -896,10 +833,10 @@
     <mergeCell ref="A1:F5"/>
     <mergeCell ref="G1:G5"/>
     <mergeCell ref="H1:O5"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="H17:K17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>